<commit_message>
updated requirements stack and added worklog excel
</commit_message>
<xml_diff>
--- a/documentation/EECS 581 Project 3 Requirements.xlsx
+++ b/documentation/EECS 581 Project 3 Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kansas-my.sharepoint.com/personal/a137p131_home_ku_edu/Documents/Year 4/Semester 1/EECS 581/Project 3/EECS-581-Project-3/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{01F59F1F-A451-FD42-B22B-AFC20DB5A1C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79735B82-A8C1-407C-B7FD-D334A7714D48}"/>
+  <xr:revisionPtr revIDLastSave="82" documentId="8_{01F59F1F-A451-FD42-B22B-AFC20DB5A1C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A1E686D-F82B-402A-8EA1-717DFBC2A0F3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="-5070" windowWidth="16440" windowHeight="29040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Stack" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>REQUIREMENTS STACK:</t>
   </si>
@@ -77,9 +77,6 @@
     <t>NPC functions (move, shoot, etc)</t>
   </si>
   <si>
-    <t>NPC types ("A.I." decisions)</t>
-  </si>
-  <si>
     <t>Basic code architecture (classes and inheritance structure)</t>
   </si>
   <si>
@@ -95,9 +92,6 @@
     <t>Game map layout</t>
   </si>
   <si>
-    <t>Main menu</t>
-  </si>
-  <si>
     <t>Player art</t>
   </si>
   <si>
@@ -128,7 +122,28 @@
     <t>In Progress</t>
   </si>
   <si>
-    <t>Not Started</t>
+    <t>Easy difficulty NPC</t>
+  </si>
+  <si>
+    <t>Medium difficulty NPC</t>
+  </si>
+  <si>
+    <t>Hard difficulty NPC</t>
+  </si>
+  <si>
+    <t>Start menu</t>
+  </si>
+  <si>
+    <t>Options menu</t>
+  </si>
+  <si>
+    <t>Game type menu (PvE or PvP)</t>
+  </si>
+  <si>
+    <t>PvE menu</t>
+  </si>
+  <si>
+    <t>PvP menu</t>
   </si>
 </sst>
 </file>
@@ -222,6 +237,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -428,7 +447,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -468,7 +487,7 @@
         <v>5</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -488,11 +507,12 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
+        <f>A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -508,11 +528,12 @@
         <v>1</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
+        <f t="shared" ref="A5:A29" si="0">A4+1</f>
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -528,11 +549,12 @@
         <v>1</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -548,11 +570,12 @@
         <v>1</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -570,6 +593,7 @@
     </row>
     <row r="8" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -587,6 +611,7 @@
     </row>
     <row r="9" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -602,11 +627,12 @@
         <v>1</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -624,13 +650,14 @@
     </row>
     <row r="11" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C11" s="2">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D11" s="3">
         <v>2</v>
@@ -641,10 +668,11 @@
     </row>
     <row r="12" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C12" s="2">
         <v>5</v>
@@ -653,41 +681,37 @@
         <v>2</v>
       </c>
       <c r="E12" s="2">
-        <v>1</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>30</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C13" s="2">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D13" s="3">
         <v>2</v>
       </c>
-      <c r="E13" s="4">
-        <v>1</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>31</v>
+      <c r="E13" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C14" s="2">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D14" s="3">
         <v>2</v>
@@ -696,52 +720,61 @@
         <v>1</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C15" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D15" s="3">
-        <v>3</v>
-      </c>
-      <c r="E15" s="2">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="E15" s="4">
+        <v>1</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C16" s="2">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D16" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E16" s="2">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C17" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" s="3">
         <v>3</v>
@@ -752,13 +785,14 @@
     </row>
     <row r="18" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C18" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D18" s="3">
         <v>3</v>
@@ -769,13 +803,14 @@
     </row>
     <row r="19" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C19" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D19" s="3">
         <v>3</v>
@@ -786,33 +821,35 @@
     </row>
     <row r="20" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="C20" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D20" s="3">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E20" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C21" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D21" s="3">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E21" s="2">
         <v>3</v>
@@ -820,48 +857,158 @@
     </row>
     <row r="22" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C22" s="2">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="D22" s="3">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="E22" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="2">
+        <v>3</v>
+      </c>
+      <c r="D23" s="3">
+        <v>20</v>
+      </c>
+      <c r="E23" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="2">
+        <v>3</v>
+      </c>
+      <c r="D24" s="3">
+        <v>3</v>
+      </c>
+      <c r="E24" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="2">
+        <v>3</v>
+      </c>
+      <c r="D25" s="3">
+        <v>3</v>
+      </c>
+      <c r="E25" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="2">
+        <v>3</v>
+      </c>
+      <c r="D26" s="3">
+        <v>10</v>
+      </c>
+      <c r="E26" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="3">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="2">
+        <v>5</v>
+      </c>
+      <c r="D27" s="3">
+        <v>10</v>
+      </c>
+      <c r="E27" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="3">
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="C23" s="3">
-        <v>2</v>
-      </c>
-      <c r="D23" s="2">
-        <v>1</v>
-      </c>
-      <c r="E23" s="3">
-        <v>1</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>30</v>
+      <c r="B28" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="2">
+        <v>21</v>
+      </c>
+      <c r="D28" s="3">
+        <v>20</v>
+      </c>
+      <c r="E28" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="3">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="3">
+        <v>2</v>
+      </c>
+      <c r="D29" s="2">
+        <v>1</v>
+      </c>
+      <c r="E29" s="3">
+        <v>1</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B32" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C32" s="4">
-        <f>SUM(C3:C22)</f>
-        <v>110</v>
+        <f>SUM(C3:C29)</f>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated sprint requirements progress levels. Created sprint 3 requirements artifacts (needs review). Updated worklog.
</commit_message>
<xml_diff>
--- a/documentation/EECS 581 Project 3 Requirements.xlsx
+++ b/documentation/EECS 581 Project 3 Requirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kansas-my.sharepoint.com/personal/a137p131_home_ku_edu/Documents/Year 4/Semester 1/EECS 581/Project 3/EECS-581-Project-3/documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kansas-my.sharepoint.com/personal/a137p131_home_ku_edu/Documents/Year 4/Semester 1/EECS 581/Project 3/EECS-581-Project-3-Sprint-2/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="8_{01F59F1F-A451-FD42-B22B-AFC20DB5A1C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A1E686D-F82B-402A-8EA1-717DFBC2A0F3}"/>
+  <xr:revisionPtr revIDLastSave="103" documentId="8_{01F59F1F-A451-FD42-B22B-AFC20DB5A1C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76B5ADD8-D65C-47B0-86F8-52C5875C7CD2}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-5070" windowWidth="16440" windowHeight="29040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16305" yWindow="-4950" windowWidth="16410" windowHeight="14505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Stack" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
   <si>
     <t>REQUIREMENTS STACK:</t>
   </si>
@@ -119,38 +119,38 @@
     <t>Completed</t>
   </si>
   <si>
+    <t>Easy difficulty NPC</t>
+  </si>
+  <si>
+    <t>Medium difficulty NPC</t>
+  </si>
+  <si>
+    <t>Hard difficulty NPC</t>
+  </si>
+  <si>
+    <t>Start menu</t>
+  </si>
+  <si>
+    <t>Options menu</t>
+  </si>
+  <si>
+    <t>Game type menu (PvE or PvP)</t>
+  </si>
+  <si>
+    <t>PvE menu</t>
+  </si>
+  <si>
+    <t>PvP menu</t>
+  </si>
+  <si>
     <t>In Progress</t>
-  </si>
-  <si>
-    <t>Easy difficulty NPC</t>
-  </si>
-  <si>
-    <t>Medium difficulty NPC</t>
-  </si>
-  <si>
-    <t>Hard difficulty NPC</t>
-  </si>
-  <si>
-    <t>Start menu</t>
-  </si>
-  <si>
-    <t>Options menu</t>
-  </si>
-  <si>
-    <t>Game type menu (PvE or PvP)</t>
-  </si>
-  <si>
-    <t>PvE menu</t>
-  </si>
-  <si>
-    <t>PvP menu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -188,6 +188,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -209,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -222,6 +229,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,7 +455,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -570,7 +578,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -608,6 +616,9 @@
       <c r="E8" s="2">
         <v>2</v>
       </c>
+      <c r="F8" s="8" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
@@ -647,6 +658,9 @@
       <c r="E10" s="2">
         <v>2</v>
       </c>
+      <c r="F10" s="7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
@@ -654,7 +668,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="2">
         <v>2</v>
@@ -664,6 +678,9 @@
       </c>
       <c r="E11" s="2">
         <v>2</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -672,7 +689,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" s="2">
         <v>5</v>
@@ -683,6 +700,9 @@
       <c r="E12" s="2">
         <v>2</v>
       </c>
+      <c r="F12" s="7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
@@ -690,7 +710,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" s="2">
         <v>3</v>
@@ -700,6 +720,9 @@
       </c>
       <c r="E13" s="2">
         <v>2</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -782,6 +805,9 @@
       <c r="E17" s="2">
         <v>2</v>
       </c>
+      <c r="F17" s="7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="18" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
@@ -800,6 +826,9 @@
       <c r="E18" s="2">
         <v>2</v>
       </c>
+      <c r="F18" s="8" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="19" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
@@ -807,7 +836,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" s="2">
         <v>1</v>
@@ -817,6 +846,9 @@
       </c>
       <c r="E19" s="2">
         <v>2</v>
+      </c>
+      <c r="F19" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -825,7 +857,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20" s="2">
         <v>2</v>
@@ -835,6 +867,9 @@
       </c>
       <c r="E20" s="2">
         <v>2</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -843,7 +878,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" s="2">
         <v>1</v>
@@ -861,7 +896,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" s="2">
         <v>1</v>
@@ -871,6 +906,9 @@
       </c>
       <c r="E22" s="2">
         <v>2</v>
+      </c>
+      <c r="F22" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -879,7 +917,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C23" s="2">
         <v>3</v>
@@ -908,6 +946,9 @@
       <c r="E24" s="2">
         <v>2</v>
       </c>
+      <c r="F24" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
@@ -925,6 +966,9 @@
       </c>
       <c r="E25" s="2">
         <v>2</v>
+      </c>
+      <c r="F25" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added support for round win buttons and switching between levels
</commit_message>
<xml_diff>
--- a/documentation/EECS 581 Project 3 Requirements.xlsx
+++ b/documentation/EECS 581 Project 3 Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kansas-my.sharepoint.com/personal/a137p131_home_ku_edu/Documents/Year 4/Semester 1/EECS 581/Project 3/EECS-581-Project-3-Sprint-2/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="103" documentId="8_{01F59F1F-A451-FD42-B22B-AFC20DB5A1C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76B5ADD8-D65C-47B0-86F8-52C5875C7CD2}"/>
+  <xr:revisionPtr revIDLastSave="113" documentId="8_{01F59F1F-A451-FD42-B22B-AFC20DB5A1C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44628DF8-2783-4706-B0A9-B8B6116DAF12}"/>
   <bookViews>
-    <workbookView xWindow="-16305" yWindow="-4950" windowWidth="16410" windowHeight="14505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2865" yWindow="4005" windowWidth="16410" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Stack" sheetId="1" r:id="rId1"/>
@@ -150,7 +150,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -190,6 +190,12 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -216,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -230,6 +236,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,7 +462,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -616,7 +623,7 @@
       <c r="E8" s="2">
         <v>2</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="9" t="s">
         <v>36</v>
       </c>
     </row>
@@ -722,7 +729,7 @@
         <v>2</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -827,7 +834,7 @@
         <v>2</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -869,7 +876,7 @@
         <v>2</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updated work log again. Added functionality to difficulty buttons. Added functionality to loss screen menu buttons. Fixed option menu return button. Fixed global variables so that they reset when new game starts
</commit_message>
<xml_diff>
--- a/documentation/EECS 581 Project 3 Requirements.xlsx
+++ b/documentation/EECS 581 Project 3 Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kansas-my.sharepoint.com/personal/a137p131_home_ku_edu/Documents/Year 4/Semester 1/EECS 581/Project 3/EECS-581-Project-3-Sprint-2/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="113" documentId="8_{01F59F1F-A451-FD42-B22B-AFC20DB5A1C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44628DF8-2783-4706-B0A9-B8B6116DAF12}"/>
+  <xr:revisionPtr revIDLastSave="115" documentId="8_{01F59F1F-A451-FD42-B22B-AFC20DB5A1C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1B9C3C3-89AD-4C67-B3E4-69555C90FE64}"/>
   <bookViews>
-    <workbookView xWindow="2865" yWindow="4005" windowWidth="16410" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Stack" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
   <si>
     <t>REQUIREMENTS STACK:</t>
   </si>
@@ -141,16 +141,13 @@
   </si>
   <si>
     <t>PvP menu</t>
-  </si>
-  <si>
-    <t>In Progress</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -194,13 +191,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -222,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -236,7 +226,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,7 +451,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -623,8 +612,8 @@
       <c r="E8" s="2">
         <v>2</v>
       </c>
-      <c r="F8" s="9" t="s">
-        <v>36</v>
+      <c r="F8" s="8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated final sprint documentation
</commit_message>
<xml_diff>
--- a/documentation/EECS 581 Project 3 Requirements.xlsx
+++ b/documentation/EECS 581 Project 3 Requirements.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28318"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kansas-my.sharepoint.com/personal/a137p131_home_ku_edu/Documents/Year 4/Semester 1/EECS 581/Project 3/EECS-581-Project-3-Sprint-2/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="115" documentId="8_{01F59F1F-A451-FD42-B22B-AFC20DB5A1C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1B9C3C3-89AD-4C67-B3E4-69555C90FE64}"/>
+  <xr:revisionPtr revIDLastSave="143" documentId="8_{01F59F1F-A451-FD42-B22B-AFC20DB5A1C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7CA6322-2FC1-4B35-875D-2F987A204E9B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Stack" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
   <si>
     <t>REQUIREMENTS STACK:</t>
   </si>
@@ -53,9 +56,15 @@
     <t>Sprint Number</t>
   </si>
   <si>
+    <t>Status</t>
+  </si>
+  <si>
     <t>Choose language/game engine</t>
   </si>
   <si>
+    <t>Completed</t>
+  </si>
+  <si>
     <t>Learn language/game engine (if necessary)</t>
   </si>
   <si>
@@ -77,6 +86,15 @@
     <t>NPC functions (move, shoot, etc)</t>
   </si>
   <si>
+    <t>Easy difficulty NPC</t>
+  </si>
+  <si>
+    <t>Medium difficulty NPC</t>
+  </si>
+  <si>
+    <t>Hard difficulty NPC</t>
+  </si>
+  <si>
     <t>Basic code architecture (classes and inheritance structure)</t>
   </si>
   <si>
@@ -92,6 +110,21 @@
     <t>Game map layout</t>
   </si>
   <si>
+    <t>Start menu</t>
+  </si>
+  <si>
+    <t>Options menu</t>
+  </si>
+  <si>
+    <t>Game type menu (PvE or PvP)</t>
+  </si>
+  <si>
+    <t>PvE menu</t>
+  </si>
+  <si>
+    <t>PvP menu</t>
+  </si>
+  <si>
     <t>Player art</t>
   </si>
   <si>
@@ -104,50 +137,29 @@
     <t>Sound effects</t>
   </si>
   <si>
-    <t>Special actions (super shot, triple shot, etc) powerups</t>
+    <t>Super shot power</t>
+  </si>
+  <si>
+    <t>Triple shot power</t>
+  </si>
+  <si>
+    <t>Speed up power</t>
+  </si>
+  <si>
+    <t>Overall Polishing</t>
   </si>
   <si>
     <t>Decide on theme</t>
   </si>
   <si>
     <t>Total story points estimated:</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Completed</t>
-  </si>
-  <si>
-    <t>Easy difficulty NPC</t>
-  </si>
-  <si>
-    <t>Medium difficulty NPC</t>
-  </si>
-  <si>
-    <t>Hard difficulty NPC</t>
-  </si>
-  <si>
-    <t>Start menu</t>
-  </si>
-  <si>
-    <t>Options menu</t>
-  </si>
-  <si>
-    <t>Game type menu (PvE or PvP)</t>
-  </si>
-  <si>
-    <t>PvE menu</t>
-  </si>
-  <si>
-    <t>PvP menu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -241,10 +253,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -448,13 +456,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="15.85546875" customWidth="1"/>
     <col min="2" max="2" width="50" customWidth="1"/>
@@ -464,7 +472,7 @@
     <col min="6" max="6" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -474,7 +482,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="12.75">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -491,15 +499,15 @@
         <v>5</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="12.75">
       <c r="A3" s="3">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
@@ -511,16 +519,16 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="12.75">
       <c r="A4" s="3">
         <f>A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C4" s="3">
         <v>8</v>
@@ -532,16 +540,16 @@
         <v>1</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="12.75">
       <c r="A5" s="3">
-        <f t="shared" ref="A5:A29" si="0">A4+1</f>
+        <f t="shared" ref="A5:A28" si="0">A4+1</f>
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
@@ -553,16 +561,16 @@
         <v>1</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="12.75">
       <c r="A6" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
@@ -574,16 +582,16 @@
         <v>1</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="12.75">
       <c r="A7" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C7" s="2">
         <v>13</v>
@@ -594,14 +602,17 @@
       <c r="E7" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="12.75">
       <c r="A8" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C8" s="2">
         <v>2</v>
@@ -613,16 +624,16 @@
         <v>2</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="12.75">
       <c r="A9" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C9" s="2">
         <v>5</v>
@@ -634,16 +645,16 @@
         <v>1</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="12.75">
       <c r="A10" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C10" s="2">
         <v>5</v>
@@ -655,16 +666,16 @@
         <v>2</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="12.75">
       <c r="A11" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C11" s="2">
         <v>2</v>
@@ -676,16 +687,16 @@
         <v>2</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="12.75">
       <c r="A12" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C12" s="2">
         <v>5</v>
@@ -697,16 +708,16 @@
         <v>2</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="18.75" customHeight="1">
       <c r="A13" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C13" s="2">
         <v>3</v>
@@ -718,16 +729,16 @@
         <v>2</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="17.25" customHeight="1">
       <c r="A14" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C14" s="2">
         <v>5</v>
@@ -739,16 +750,16 @@
         <v>1</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="12.75">
       <c r="A15" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C15" s="2">
         <v>8</v>
@@ -760,16 +771,16 @@
         <v>1</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="12.75">
       <c r="A16" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C16" s="2">
         <v>13</v>
@@ -781,79 +792,79 @@
         <v>1</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="12.75">
       <c r="A17" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2</v>
+      </c>
+      <c r="D17" s="3">
+        <v>3</v>
+      </c>
+      <c r="E17" s="2">
+        <v>2</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="12.75">
+      <c r="A18" s="3">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="2">
+        <v>2</v>
+      </c>
+      <c r="D18" s="3">
+        <v>3</v>
+      </c>
+      <c r="E18" s="2">
+        <v>2</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="12.75">
+      <c r="A19" s="3">
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C17" s="2">
-        <v>2</v>
-      </c>
-      <c r="D17" s="3">
-        <v>3</v>
-      </c>
-      <c r="E17" s="2">
-        <v>2</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="3">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B18" s="2" t="s">
+      <c r="B19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3">
+        <v>3</v>
+      </c>
+      <c r="E19" s="2">
+        <v>2</v>
+      </c>
+      <c r="F19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="12.75">
+      <c r="A20" s="3">
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C18" s="2">
-        <v>2</v>
-      </c>
-      <c r="D18" s="3">
-        <v>3</v>
-      </c>
-      <c r="E18" s="2">
-        <v>2</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="3">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="2">
-        <v>1</v>
-      </c>
-      <c r="D19" s="3">
-        <v>3</v>
-      </c>
-      <c r="E19" s="2">
-        <v>2</v>
-      </c>
-      <c r="F19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="3">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
       <c r="B20" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C20" s="2">
         <v>2</v>
@@ -865,16 +876,16 @@
         <v>2</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="12.75">
       <c r="A21" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C21" s="2">
         <v>1</v>
@@ -885,14 +896,17 @@
       <c r="E21" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="12.75">
       <c r="A22" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C22" s="2">
         <v>1</v>
@@ -904,16 +918,16 @@
         <v>2</v>
       </c>
       <c r="F22" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="12.75">
       <c r="A23" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C23" s="2">
         <v>3</v>
@@ -924,14 +938,17 @@
       <c r="E23" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1">
       <c r="A24" s="3">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C24" s="2">
         <v>3</v>
@@ -943,16 +960,16 @@
         <v>2</v>
       </c>
       <c r="F24" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1">
       <c r="A25" s="3">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C25" s="2">
         <v>3</v>
@@ -964,16 +981,16 @@
         <v>2</v>
       </c>
       <c r="F25" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1">
       <c r="A26" s="3">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C26" s="2">
         <v>3</v>
@@ -984,14 +1001,17 @@
       <c r="E26" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1">
       <c r="A27" s="3">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C27" s="2">
         <v>5</v>
@@ -1002,17 +1022,20 @@
       <c r="E27" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1">
       <c r="A28" s="3">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="C28" s="2">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D28" s="3">
         <v>20</v>
@@ -1021,34 +1044,84 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="3">
-        <f t="shared" si="0"/>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A29">
         <v>27</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" s="3">
-        <v>2</v>
-      </c>
-      <c r="D29" s="2">
-        <v>1</v>
-      </c>
-      <c r="E29" s="3">
-        <v>1</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B32" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" s="4">
-        <f>SUM(C3:C29)</f>
-        <v>121</v>
+      <c r="B29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29">
+        <v>7</v>
+      </c>
+      <c r="D29">
+        <v>20</v>
+      </c>
+      <c r="E29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30">
+        <v>7</v>
+      </c>
+      <c r="D30">
+        <v>20</v>
+      </c>
+      <c r="E30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31">
+        <v>7</v>
+      </c>
+      <c r="D31">
+        <v>10</v>
+      </c>
+      <c r="E31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="12.75">
+      <c r="A32" s="3">
+        <v>29</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="3">
+        <v>2</v>
+      </c>
+      <c r="D32" s="2">
+        <v>1</v>
+      </c>
+      <c r="E32" s="3">
+        <v>1</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B34" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="4">
+        <f>SUM(C3:C32)</f>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>